<commit_message>
Add basic information in scrum planning
</commit_message>
<xml_diff>
--- a/Scrum planning.xlsx
+++ b/Scrum planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elive\OneDrive - AP Hogeschool Antwerpen\2de Jaar IT\semester 2\Security project\6\securityProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\securityProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F562F9BE-4E00-465C-BE4D-8E1BBACDBCCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06E7A01-8C10-40D9-B368-CFAC313FEF02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E07F6153-1B8C-43A7-97BD-457FD435295E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{E07F6153-1B8C-43A7-97BD-457FD435295E}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="86">
   <si>
     <t>Naam</t>
   </si>
@@ -252,6 +252,54 @@
   </si>
   <si>
     <t>Monowal Shrestha</t>
+  </si>
+  <si>
+    <t>Infromatie opzoeken rond RSS</t>
+  </si>
+  <si>
+    <t>Infromatie opzoeken rond DNS</t>
+  </si>
+  <si>
+    <t>Voltooid</t>
+  </si>
+  <si>
+    <t>Een eerste versie hebben van de frontend</t>
+  </si>
+  <si>
+    <t>Maken van API</t>
+  </si>
+  <si>
+    <t>Maken van Angrular frontend</t>
+  </si>
+  <si>
+    <t>DNS op rocky linux</t>
+  </si>
+  <si>
+    <t>De DNS op rocky was de eerste oplossing, we hebben hierna voor een andere oplossing rond dns gekozen</t>
+  </si>
+  <si>
+    <t>Dockerize frontend en API</t>
+  </si>
+  <si>
+    <t>Pihole</t>
+  </si>
+  <si>
+    <t>Cloudflared</t>
+  </si>
+  <si>
+    <t>Live changes Angular</t>
+  </si>
+  <si>
+    <t>Frontend styling</t>
+  </si>
+  <si>
+    <t>Search pagina angular</t>
+  </si>
+  <si>
+    <t>Filtering</t>
+  </si>
+  <si>
+    <t>Documentatie</t>
   </si>
 </sst>
 </file>
@@ -533,11 +581,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -547,11 +600,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1084,9 +1132,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Thema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1124,7 +1172,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1230,7 +1278,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1372,7 +1420,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1382,20 +1430,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2DE5DA5-9F86-4F5C-B1E1-90B69129D774}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="159" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.109375" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="14" t="s">
         <v>20</v>
       </c>
@@ -1408,29 +1456,29 @@
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
     </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="16"/>
     </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="17"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D4" s="18"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>61</v>
       </c>
@@ -1441,7 +1489,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>62</v>
       </c>
@@ -1450,10 +1498,10 @@
       </c>
       <c r="D8">
         <f>'Sprint 1'!$F$31+'Sprint 2'!$F$31+'Sprint 3'!$F$31+'Sprint 4'!$F$31+'Sprint 5'!$F$31+'Sprint 6'!$F$31+'Sprint 7'!$F$31</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>63</v>
       </c>
@@ -1465,7 +1513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>64</v>
       </c>
@@ -1477,7 +1525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>65</v>
       </c>
@@ -1486,12 +1534,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1502,7 +1550,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>9</v>
       </c>
@@ -1515,7 +1563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>10</v>
       </c>
@@ -1528,7 +1576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>11</v>
       </c>
@@ -1541,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>24</v>
       </c>
@@ -1579,19 +1627,19 @@
       <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" customWidth="1"/>
-    <col min="3" max="3" width="47.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="47.140625" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="14" t="s">
         <v>12</v>
       </c>
@@ -1604,12 +1652,12 @@
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -1641,7 +1689,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1655,27 +1703,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K7" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K10" t="s">
         <v>29</v>
       </c>
@@ -1705,20 +1753,21 @@
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B36:J36"/>
+      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="4" max="5" width="17.77734375" customWidth="1"/>
-    <col min="6" max="9" width="10.77734375" customWidth="1"/>
-    <col min="10" max="10" width="35.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="14" t="s">
         <v>19</v>
       </c>
@@ -1732,7 +1781,7 @@
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>33</v>
       </c>
@@ -1746,63 +1795,63 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="10"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="10"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-    </row>
-    <row r="12" spans="1:10" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-    </row>
-    <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+    </row>
+    <row r="12" spans="1:10" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+    </row>
+    <row r="14" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>32</v>
       </c>
@@ -1816,16 +1865,16 @@
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -1857,31 +1906,43 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="3">
+        <v>7</v>
+      </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1893,7 +1954,7 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1905,7 +1966,7 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1917,7 +1978,7 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1929,7 +1990,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1941,7 +2002,7 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1953,7 +2014,7 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1965,7 +2026,7 @@
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1977,7 +2038,7 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1989,7 +2050,7 @@
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -2001,7 +2062,7 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -2013,7 +2074,7 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -2025,7 +2086,7 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2035,7 +2096,7 @@
       </c>
       <c r="F31" s="5">
         <f>SUM(F17:F30)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G31" s="5">
         <f t="shared" ref="G31:I31" si="0">SUM(G17:G30)</f>
@@ -2051,7 +2112,7 @@
       </c>
       <c r="J31" s="5"/>
     </row>
-    <row r="33" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>39</v>
       </c>
@@ -2065,164 +2126,170 @@
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="24"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="27"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="19"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="20"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
-      <c r="J37" s="19"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="20"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="19"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="20"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="19"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="20"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="19"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="20"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="19"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="20"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="19"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="20"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="19"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="20"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
-      <c r="J44" s="19"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="20"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="26"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="B35:J35"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="B45:J45"/>
@@ -2232,12 +2299,6 @@
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="B42:J42"/>
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="B35:J35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2250,22 +2311,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE36C8E1-C9DA-45BD-B73B-7521063AD367}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="4" max="5" width="17.77734375" customWidth="1"/>
-    <col min="6" max="9" width="10.77734375" customWidth="1"/>
-    <col min="10" max="10" width="35.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="14" t="s">
         <v>52</v>
       </c>
@@ -2279,7 +2340,7 @@
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>33</v>
       </c>
@@ -2293,63 +2354,65 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="10"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="10"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-    </row>
-    <row r="12" spans="1:10" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-    </row>
-    <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+    </row>
+    <row r="12" spans="1:10" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+    </row>
+    <row r="14" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>32</v>
       </c>
@@ -2363,16 +2426,16 @@
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -2404,9 +2467,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -2416,9 +2481,11 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -2428,19 +2495,25 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
+      <c r="B19" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="F19" s="3">
+        <v>7</v>
+      </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2452,7 +2525,7 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2464,7 +2537,7 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2476,7 +2549,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -2488,7 +2561,7 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -2500,7 +2573,7 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2512,7 +2585,7 @@
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2524,7 +2597,7 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -2536,7 +2609,7 @@
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -2548,7 +2621,7 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -2560,7 +2633,7 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -2572,7 +2645,7 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2582,7 +2655,7 @@
       </c>
       <c r="F31" s="5">
         <f>SUM(F17:F30)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G31" s="5">
         <f t="shared" ref="G31:I31" si="0">SUM(G17:G30)</f>
@@ -2598,7 +2671,7 @@
       </c>
       <c r="J31" s="5"/>
     </row>
-    <row r="33" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>39</v>
       </c>
@@ -2612,164 +2685,172 @@
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="24"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="27"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="19"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B36" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="20"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
-      <c r="J37" s="19"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="20"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="19"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="20"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="19"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="20"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="19"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="20"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="19"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="20"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="19"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="20"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="19"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="20"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
-      <c r="J44" s="19"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="20"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="26"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B35:J35"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="B45:J45"/>
@@ -2779,12 +2860,6 @@
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="B42:J42"/>
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B35:J35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2799,20 +2874,20 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="4" max="5" width="17.77734375" customWidth="1"/>
-    <col min="6" max="9" width="10.77734375" customWidth="1"/>
-    <col min="10" max="10" width="35.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="14" t="s">
         <v>54</v>
       </c>
@@ -2826,7 +2901,7 @@
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>33</v>
       </c>
@@ -2840,63 +2915,63 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="10"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="10"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-    </row>
-    <row r="12" spans="1:10" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-    </row>
-    <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+    </row>
+    <row r="12" spans="1:10" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+    </row>
+    <row r="14" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>32</v>
       </c>
@@ -2910,16 +2985,16 @@
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -2951,9 +3026,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -2963,9 +3040,11 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -2975,7 +3054,7 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2987,7 +3066,7 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2999,7 +3078,7 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -3011,7 +3090,7 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -3023,7 +3102,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -3035,7 +3114,7 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -3047,7 +3126,7 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -3059,7 +3138,7 @@
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -3071,7 +3150,7 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -3083,7 +3162,7 @@
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -3095,7 +3174,7 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -3107,7 +3186,7 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -3119,7 +3198,7 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -3145,7 +3224,7 @@
       </c>
       <c r="J31" s="5"/>
     </row>
-    <row r="33" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>39</v>
       </c>
@@ -3159,164 +3238,170 @@
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="24"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="27"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="19"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="20"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
-      <c r="J37" s="19"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="20"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="19"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="20"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="19"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="20"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="19"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="20"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="19"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="20"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="19"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="20"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="19"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="20"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
-      <c r="J44" s="19"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="20"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="26"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B35:J35"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="B45:J45"/>
@@ -3326,12 +3411,6 @@
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="B42:J42"/>
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B35:J35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3346,20 +3425,20 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="4" max="5" width="17.77734375" customWidth="1"/>
-    <col min="6" max="9" width="10.77734375" customWidth="1"/>
-    <col min="10" max="10" width="35.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="14" t="s">
         <v>53</v>
       </c>
@@ -3373,7 +3452,7 @@
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>33</v>
       </c>
@@ -3387,63 +3466,63 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="10"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="10"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-    </row>
-    <row r="12" spans="1:10" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-    </row>
-    <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+    </row>
+    <row r="12" spans="1:10" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+    </row>
+    <row r="14" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>32</v>
       </c>
@@ -3457,16 +3536,16 @@
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -3498,9 +3577,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -3510,9 +3591,11 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -3522,9 +3605,11 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
+      <c r="B19" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -3534,7 +3619,7 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -3546,7 +3631,7 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -3558,7 +3643,7 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -3570,7 +3655,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -3582,7 +3667,7 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -3594,7 +3679,7 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -3606,7 +3691,7 @@
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -3618,7 +3703,7 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -3630,7 +3715,7 @@
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -3642,7 +3727,7 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -3654,7 +3739,7 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -3666,7 +3751,7 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -3692,7 +3777,7 @@
       </c>
       <c r="J31" s="5"/>
     </row>
-    <row r="33" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>39</v>
       </c>
@@ -3706,164 +3791,170 @@
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="24"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="27"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="19"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="20"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
-      <c r="J37" s="19"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="20"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="19"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="20"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="19"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="20"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="19"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="20"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="19"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="20"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="19"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="20"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="19"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="20"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
-      <c r="J44" s="19"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="20"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="26"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B35:J35"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="B45:J45"/>
@@ -3873,12 +3964,6 @@
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="B42:J42"/>
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B35:J35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3893,20 +3978,20 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="4" max="5" width="17.77734375" customWidth="1"/>
-    <col min="6" max="9" width="10.77734375" customWidth="1"/>
-    <col min="10" max="10" width="35.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="14" t="s">
         <v>55</v>
       </c>
@@ -3920,7 +4005,7 @@
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>33</v>
       </c>
@@ -3934,63 +4019,63 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="10"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="10"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-    </row>
-    <row r="12" spans="1:10" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-    </row>
-    <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+    </row>
+    <row r="12" spans="1:10" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+    </row>
+    <row r="14" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>32</v>
       </c>
@@ -4004,16 +4089,16 @@
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -4045,9 +4130,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -4057,7 +4144,7 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -4069,7 +4156,7 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -4081,7 +4168,7 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -4093,7 +4180,7 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -4105,7 +4192,7 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -4117,7 +4204,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -4129,7 +4216,7 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -4141,7 +4228,7 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -4153,7 +4240,7 @@
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -4165,7 +4252,7 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -4177,7 +4264,7 @@
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -4189,7 +4276,7 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -4201,7 +4288,7 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -4213,7 +4300,7 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -4239,7 +4326,7 @@
       </c>
       <c r="J31" s="5"/>
     </row>
-    <row r="33" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>39</v>
       </c>
@@ -4253,164 +4340,170 @@
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="24"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="27"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="19"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="20"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
-      <c r="J37" s="19"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="20"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="19"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="20"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="19"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="20"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="19"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="20"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="19"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="20"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="19"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="20"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="19"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="20"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
-      <c r="J44" s="19"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="20"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="26"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B35:J35"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="B45:J45"/>
@@ -4420,12 +4513,6 @@
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="B42:J42"/>
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B35:J35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -4440,20 +4527,20 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="4" max="5" width="17.77734375" customWidth="1"/>
-    <col min="6" max="9" width="10.77734375" customWidth="1"/>
-    <col min="10" max="10" width="35.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="14" t="s">
         <v>56</v>
       </c>
@@ -4467,7 +4554,7 @@
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>33</v>
       </c>
@@ -4481,63 +4568,63 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="10"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="10"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-    </row>
-    <row r="12" spans="1:10" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-    </row>
-    <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+    </row>
+    <row r="12" spans="1:10" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+    </row>
+    <row r="14" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>32</v>
       </c>
@@ -4551,16 +4638,16 @@
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -4592,9 +4679,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -4604,9 +4693,11 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -4616,7 +4707,7 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -4628,7 +4719,7 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -4640,7 +4731,7 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -4652,7 +4743,7 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -4664,7 +4755,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -4676,7 +4767,7 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -4688,7 +4779,7 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -4700,7 +4791,7 @@
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -4712,7 +4803,7 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -4724,7 +4815,7 @@
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -4736,7 +4827,7 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -4748,7 +4839,7 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -4760,7 +4851,7 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -4786,7 +4877,7 @@
       </c>
       <c r="J31" s="5"/>
     </row>
-    <row r="33" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>39</v>
       </c>
@@ -4800,164 +4891,170 @@
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="24"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="27"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="19"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="20"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
-      <c r="J37" s="19"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="20"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="19"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="20"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="19"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="20"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="19"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="20"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="19"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="20"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="19"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="20"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="19"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="20"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
-      <c r="J44" s="19"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="20"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="26"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B35:J35"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="B45:J45"/>
@@ -4967,12 +5064,6 @@
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="B42:J42"/>
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B35:J35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -4990,17 +5081,17 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="4" max="5" width="17.77734375" customWidth="1"/>
-    <col min="6" max="9" width="10.77734375" customWidth="1"/>
-    <col min="10" max="10" width="35.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="14" t="s">
         <v>57</v>
       </c>
@@ -5014,7 +5105,7 @@
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>33</v>
       </c>
@@ -5028,63 +5119,63 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="10"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="10"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-    </row>
-    <row r="12" spans="1:10" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-    </row>
-    <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+    </row>
+    <row r="12" spans="1:10" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+    </row>
+    <row r="14" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>32</v>
       </c>
@@ -5098,16 +5189,16 @@
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -5139,7 +5230,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -5151,7 +5242,7 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -5163,7 +5254,7 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -5175,7 +5266,7 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -5187,7 +5278,7 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -5199,7 +5290,7 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -5211,7 +5302,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -5223,7 +5314,7 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -5235,7 +5326,7 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -5247,7 +5338,7 @@
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -5259,7 +5350,7 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -5271,7 +5362,7 @@
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -5283,7 +5374,7 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -5295,7 +5386,7 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -5307,7 +5398,7 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -5333,7 +5424,7 @@
       </c>
       <c r="J31" s="5"/>
     </row>
-    <row r="33" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>39</v>
       </c>
@@ -5347,164 +5438,170 @@
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="24"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="27"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="19"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="20"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
-      <c r="J37" s="19"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="20"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="19"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="20"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="19"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="20"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="19"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="20"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="19"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="20"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="19"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="20"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="19"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="20"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
-      <c r="J44" s="19"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="20"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="26"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B35:J35"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="B45:J45"/>
@@ -5514,12 +5611,6 @@
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="B42:J42"/>
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B35:J35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -5529,21 +5620,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009EB83581AE75E3448E2425BE2C4A9358" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c09722cb83f8a2755d0c5b1e3ee63688">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0967b7be50301903c78f9c39c6fd9af8">
     <xsd:element name="properties">
@@ -5657,10 +5733,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E4C23C1-DCFE-4CD3-9D30-B3FD71E92F59}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3230093E-2E26-4FBA-AA3F-A32CF67ED8B4}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
@@ -5675,16 +5773,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3230093E-2E26-4FBA-AA3F-A32CF67ED8B4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E4C23C1-DCFE-4CD3-9D30-B3FD71E92F59}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>